<commit_message>
seed 19 run for all treatments
</commit_message>
<xml_diff>
--- a/images/seed_numbers.xlsx
+++ b/images/seed_numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vavaocel/Documents/projects/heterogenous_game_theory/data_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vavaocel/Documents/projects/heterogenous_game_theory/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3B337A78-07ED-BC4E-ABC9-141FFE0A9101}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B863DCC4-DBE2-0D45-B5D7-7ADFECDE978D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="seed_numbers" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="5" uniqueCount="5">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="9" uniqueCount="6">
   <si>
     <t>seed</t>
   </si>
@@ -41,11 +41,14 @@
   <si>
     <t>power_law</t>
   </si>
+  <si>
+    <t>X</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="12"/>
@@ -523,8 +526,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -570,7 +576,29 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -584,17 +612,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" id="1" name="Table1" displayName="Table1" ref="A1:E101" totalsRowShown="0">
-  <autoFilter ref="A1:E101"/>
+<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E101" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:E101" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E101">
     <sortCondition ref="A1:A101"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="seed"/>
-    <tableColumn id="2" name="control_group"/>
-    <tableColumn id="3" name="sd_ei"/>
-    <tableColumn id="4" name="complete_hetero"/>
-    <tableColumn id="5" name="power_law"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="seed" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="control_group" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="sd_ei" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="complete_hetero" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="power_law" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -896,535 +924,548 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="23.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="23.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>19</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>243</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>268</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>296</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>303</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>304</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>311</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>320</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>323</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38">
+      <c r="A38" s="1">
         <v>333</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39">
+      <c r="A39" s="1">
         <v>365</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40">
+      <c r="A40" s="1">
         <v>391</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>397</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42">
+      <c r="A42" s="1">
         <v>402</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43">
+      <c r="A43" s="1">
         <v>417</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44">
+      <c r="A44" s="1">
         <v>424</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45">
+      <c r="A45" s="1">
         <v>435</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46">
+      <c r="A46" s="1">
         <v>440</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47">
+      <c r="A47" s="1">
         <v>440</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48">
+      <c r="A48" s="1">
         <v>447</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49">
+      <c r="A49" s="1">
         <v>474</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50">
+      <c r="A50" s="1">
         <v>487</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51">
+      <c r="A51" s="1">
         <v>502</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52">
+      <c r="A52" s="1">
         <v>508</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53">
+      <c r="A53" s="1">
         <v>519</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54">
+      <c r="A54" s="1">
         <v>521</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55">
+      <c r="A55" s="1">
         <v>524</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56">
+      <c r="A56" s="1">
         <v>531</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57">
+      <c r="A57" s="1">
         <v>558</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58">
+      <c r="A58" s="1">
         <v>562</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59">
+      <c r="A59" s="1">
         <v>575</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60">
+      <c r="A60" s="1">
         <v>596</v>
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61">
+      <c r="A61" s="1">
         <v>601</v>
       </c>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62">
+      <c r="A62" s="1">
         <v>605</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63">
+      <c r="A63" s="1">
         <v>612</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64">
+      <c r="A64" s="1">
         <v>618</v>
       </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65">
+      <c r="A65" s="1">
         <v>639</v>
       </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66">
+      <c r="A66" s="1">
         <v>649</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67">
+      <c r="A67" s="1">
         <v>652</v>
       </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68">
+      <c r="A68" s="1">
         <v>662</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69">
+      <c r="A69" s="1">
         <v>670</v>
       </c>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70">
+      <c r="A70" s="1">
         <v>683</v>
       </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71">
+      <c r="A71" s="1">
         <v>704</v>
       </c>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72">
+      <c r="A72" s="1">
         <v>706</v>
       </c>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73">
+      <c r="A73" s="1">
         <v>717</v>
       </c>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74">
+      <c r="A74" s="1">
         <v>727</v>
       </c>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75">
+      <c r="A75" s="1">
         <v>741</v>
       </c>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76">
+      <c r="A76" s="1">
         <v>745</v>
       </c>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77">
+      <c r="A77" s="1">
         <v>750</v>
       </c>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78">
+      <c r="A78" s="1">
         <v>771</v>
       </c>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79">
+      <c r="A79" s="1">
         <v>773</v>
       </c>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80">
+      <c r="A80" s="1">
         <v>774</v>
       </c>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81">
+      <c r="A81" s="1">
         <v>777</v>
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82">
+      <c r="A82" s="1">
         <v>780</v>
       </c>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83">
+      <c r="A83" s="1">
         <v>785</v>
       </c>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84">
+      <c r="A84" s="1">
         <v>795</v>
       </c>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85">
+      <c r="A85" s="1">
         <v>813</v>
       </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86">
+      <c r="A86" s="1">
         <v>818</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87">
+      <c r="A87" s="1">
         <v>819</v>
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88">
+      <c r="A88" s="1">
         <v>822</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89">
+      <c r="A89" s="1">
         <v>822</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90">
+      <c r="A90" s="1">
         <v>839</v>
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91">
+      <c r="A91" s="1">
         <v>842</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92">
+      <c r="A92" s="1">
         <v>870</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93">
+      <c r="A93" s="1">
         <v>872</v>
       </c>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94">
+      <c r="A94" s="1">
         <v>881</v>
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95">
+      <c r="A95" s="1">
         <v>899</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96">
+      <c r="A96" s="1">
         <v>920</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97">
+      <c r="A97" s="1">
         <v>938</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98">
+      <c r="A98" s="1">
         <v>944</v>
       </c>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99">
+      <c r="A99" s="1">
         <v>960</v>
       </c>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100">
+      <c r="A100" s="1">
         <v>974</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101">
+      <c r="A101" s="1">
         <v>994</v>
       </c>
     </row>

</xml_diff>